<commit_message>
thesis updated, assistant edit and delete functionality added
</commit_message>
<xml_diff>
--- a/DOC/tablas importantes/Tabla gpt3 gpt4 palm 1 y 2 y llama2.xlsx
+++ b/DOC/tablas importantes/Tabla gpt3 gpt4 palm 1 y 2 y llama2.xlsx
@@ -15,7 +15,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
-    <t xml:space="preserve">Benchmarks (Shots)</t>
+    <t xml:space="preserve">Marcos de Prueba (Intentos)</t>
   </si>
   <si>
     <t>GPT-3,5</t>
@@ -33,7 +33,7 @@
     <t xml:space="preserve">Llama 2</t>
   </si>
   <si>
-    <t xml:space="preserve">MMLU (5-shot)</t>
+    <t xml:space="preserve">MMLU (5-intentos)</t>
   </si>
   <si>
     <t xml:space="preserve">70.0 </t>
@@ -51,22 +51,22 @@
     <t>68.9</t>
   </si>
   <si>
-    <t xml:space="preserve">TriviaQA (1-shot)</t>
+    <t xml:space="preserve">TriviaQA (1-intento)</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t xml:space="preserve">Natural Questions (1-shot)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QSM8K (8-shot)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HumanEval (0-shot)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BIG-Bench Hard (3-shot)</t>
+    <t xml:space="preserve">Preguntas Naturales (1-intento)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QSM8K (8-intentos)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EvalHumana (0-intentos)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BBH (3-intentos)</t>
   </si>
 </sst>
 </file>
@@ -89,7 +89,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -97,12 +97,36 @@
       <bottom style="none"/>
       <diagonal style="none"/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -619,26 +643,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" min="1" max="1" width="17.7109375"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" width="25.140625"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -646,19 +670,19 @@
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -666,39 +690,39 @@
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>81.400000000000006</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <v>83.099999999999994</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="2">
         <v>85</v>
       </c>
     </row>
-    <row r="4" ht="14.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" ht="28.5">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>29.300000000000001</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
         <v>37.5</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="2">
         <v>33</v>
       </c>
     </row>
@@ -706,19 +730,19 @@
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>57.100000000000001</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2">
         <v>92</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>56.5</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="2">
         <v>80.700000000000003</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="2">
         <v>56.799999999999997</v>
       </c>
     </row>
@@ -726,19 +750,19 @@
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>48.100000000000001</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="2">
         <v>67</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>26.199999999999999</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="2">
         <v>29.899999999999999</v>
       </c>
     </row>
@@ -746,29 +770,29 @@
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>52.299999999999997</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="2">
         <v>65.700000000000003</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="2">
         <v>51.200000000000003</v>
       </c>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>